<commit_message>
MSEs for cv data completed
</commit_message>
<xml_diff>
--- a/Kelvin/3. Experimentation/Linear Regression Model Selection.xlsx
+++ b/Kelvin/3. Experimentation/Linear Regression Model Selection.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Kelvin\3. Experimentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\COMP 551\COMP-551-Project-1\Kelvin\3. Experimentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A7DD62-B414-4750-83CB-E8363CDEDBA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F927832F-2DB3-4D6E-9856-9437A15D815A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="10583" activeTab="1" xr2:uid="{22610710-CCF8-47BC-B229-9A9BE554869F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26985" windowHeight="10583" xr2:uid="{22610710-CCF8-47BC-B229-9A9BE554869F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Linear Regression Model Selection:</t>
   </si>
@@ -50,6 +49,18 @@
   </si>
   <si>
     <t>Dataset 5</t>
+  </si>
+  <si>
+    <t>Dataset 6</t>
+  </si>
+  <si>
+    <t>Mean Squared Errors</t>
+  </si>
+  <si>
+    <t>Number of Iterations</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -88,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -108,6 +119,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,7 +183,16 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Comparisons for Model Selection</a:t>
+              <a:t> Comparisons for </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t>Model Selection</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -211,7 +238,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet 2'!$B$3</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -232,9 +259,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet 2'!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$5:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Dataset 1</c:v>
                 </c:pt>
@@ -246,34 +273,46 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 2'!$B$4:$B$7</c:f>
+              <c:f>Sheet1!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>996.38546425768902</c:v>
+                  <c:v>0.99638546425768904</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>969.28676418401199</c:v>
+                  <c:v>0.96928676418401205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>996.25764309645797</c:v>
+                  <c:v>0.99625764309645803</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>969.21015771272903</c:v>
+                  <c:v>0.969210157712729</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02032668484314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0159737956686901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4376-4920-8644-664AF6DF519D}"/>
+              <c16:uniqueId val="{00000000-E44C-4394-ACA1-C2DECDC5A954}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -282,7 +321,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet 2'!$C$3</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -303,9 +342,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sheet 2'!$A$4:$A$7</c:f>
+              <c:f>Sheet1!$A$5:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Dataset 1</c:v>
                 </c:pt>
@@ -317,34 +356,46 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 2'!$C$4:$C$7</c:f>
+              <c:f>Sheet1!$C$5:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1529.9481660261499</c:v>
+                  <c:v>1.3339661503361799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>995.17814525392498</c:v>
+                  <c:v>1.0057968591374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6256.2497846642</c:v>
+                  <c:v>9.4297005097350706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5602.2757696978497</c:v>
+                  <c:v>6.0861178731953798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.32655617656527</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9819783427800199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4376-4920-8644-664AF6DF519D}"/>
+              <c16:uniqueId val="{00000001-E44C-4394-ACA1-C2DECDC5A954}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -592,844 +643,14 @@
               <a:rPr lang="en-CA" baseline="0"/>
               <a:t> Comparisons of Dataset 1 and 2</a:t>
             </a:r>
-            <a:endParaRPr lang="en-CA"/>
           </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet 2'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Normal Equatuion Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet 2'!$A$4:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Dataset 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dataset 2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet 2'!$B$4:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>996.38546425768902</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>969.28676418401199</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1A46-45B4-BF66-72A584AFD196}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet 2'!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Gradient Descent Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet 2'!$A$4:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Dataset 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dataset 2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet 2'!$C$4:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1529.9481660261499</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>995.17814525392498</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1A46-45B4-BF66-72A584AFD196}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="405102912"/>
-        <c:axId val="400355488"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="405102912"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="400355488"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="400355488"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="405102912"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>Mean Squared Error</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Comparisons for Model Selection</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Normal Equatuion Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Dataset 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dataset 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dataset 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Dataset 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dataset 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.99638546425768904</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.96928676418401205</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99625764309645803</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.969210157712729</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.02032668484314</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E44C-4394-ACA1-C2DECDC5A954}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Gradient Descent Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Dataset 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Dataset 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dataset 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Dataset 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dataset 5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000000000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.52994816602615</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99517814525392501</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.2562497846641998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.60227576969785</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1549039256978899</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E44C-4394-ACA1-C2DECDC5A954}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="405102584"/>
-        <c:axId val="405107832"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="405102584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="405107832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="405107832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="405102584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>MSE</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Comparisons of Dataset 1 and 2</a:t>
+              <a:t>(Prescribed Features)</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -1476,7 +697,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1497,7 +718,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$5</c:f>
+              <c:f>Sheet1!$A$5:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1511,7 +732,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$5</c:f>
+              <c:f>Sheet1!$B$5:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000000</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1535,7 +756,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1556,7 +777,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$5</c:f>
+              <c:f>Sheet1!$A$5:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1570,15 +791,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$5</c:f>
+              <c:f>Sheet1!$C$5:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.52994816602615</c:v>
+                  <c:v>1.3339661503361799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99517814525392501</c:v>
+                  <c:v>1.0057968591374</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1792,6 +1013,381 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Mean Squared Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Comparisons of </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t>Normal Equation Solutions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normal Equatuion Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$5:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Dataset 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dataset 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dataset 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.99638546425768904</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96928676418401205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99625764309645803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.969210157712729</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02032668484314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0159737956686901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F1FF-4D47-9A16-9CE4451DB1D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="405102584"/>
+        <c:axId val="405107832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="405102584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405107832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="405107832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405102584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1912,46 +1508,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2959,509 +2515,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3970,94 +3023,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1081088</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDB70E47-3800-4E1C-9EC5-D0EF8ABC17D1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2179D66-24B8-485F-9718-69AD303D6C0B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1081088</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4087,13 +3059,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4114,6 +3086,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1069182</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83794DB5-ADCC-4F2C-A395-DD9968046080}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4418,17 +3428,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EFD77A-D35B-4770-88AC-D48A47F2D144}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B66CD76-67A4-4C5B-9C2A-ECA670609720}">
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="3" width="20.265625" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.46484375" customWidth="1"/>
+    <col min="13" max="14" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -4448,176 +3459,126 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>996.38546425768902</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1529.9481660261499</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>969.28676418401199</v>
-      </c>
-      <c r="C5" s="3">
-        <v>995.17814525392498</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
-        <v>996.25764309645797</v>
-      </c>
-      <c r="C6" s="3">
-        <v>6256.2497846642</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3">
-        <v>969.21015771272903</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5602.2757696978497</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B66CD76-67A4-4C5B-9C2A-ECA670609720}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="3" width="20.265625" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.99638546425768904</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.52994816602615</v>
-      </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.96928676418401205</v>
+      <c r="B5" s="2">
+        <v>0.99638546425768904</v>
       </c>
-      <c r="C5" s="3">
-        <v>0.99517814525392501</v>
+      <c r="C5" s="2">
+        <v>1.3339661503361799</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="D5" s="8">
+        <v>165586</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>0.99625764309645803</v>
+        <v>0.96928676418401205</v>
       </c>
       <c r="C6" s="3">
-        <v>6.2562497846641998</v>
+        <v>1.0057968591374</v>
+      </c>
+      <c r="D6" s="9">
+        <v>84717</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>0.969210157712729</v>
+        <v>0.99625764309645803</v>
       </c>
       <c r="C7" s="3">
-        <v>5.60227576969785</v>
+        <v>9.4297005097350706</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3985002</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>1.02032668484314</v>
+        <v>0.969210157712729</v>
       </c>
       <c r="C8" s="3">
-        <v>2.1549039256978899</v>
+        <v>6.0861178731953798</v>
+      </c>
+      <c r="D8" s="9">
+        <v>3226422</v>
       </c>
       <c r="E8" s="3"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.02032668484314</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3.32655617656527</v>
+      </c>
+      <c r="D9" s="9">
+        <v>4101608</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.0159737956686901</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.9819783427800199</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2233762</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>